<commit_message>
modified:   EXPORTACIONESDEFRESA.ipynb 	modified:   "Exportaciones-agr\303\255colas-no-tradicionales-y-tradicionales (1).xlsx"
</commit_message>
<xml_diff>
--- a/Exportaciones-agrícolas-no-tradicionales-y-tradicionales (1).xlsx
+++ b/Exportaciones-agrícolas-no-tradicionales-y-tradicionales (1).xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alzat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alzat\OneDrive\Documentos\Desafio1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A6AEC8-E015-4D4D-8235-6E34E1FA25D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736EE6BA-B76C-4B49-B734-55CB3849AED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DATA!$A$1:$M$103</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -152,11 +152,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\ mmm\ dd\ hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="#,##0.###########"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +168,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -190,16 +199,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,12 +523,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="13" width="30.85546875" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -551,10 +567,10 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -592,10 +608,10 @@
       <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="5">
         <v>34</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="5">
         <v>13</v>
       </c>
     </row>
@@ -633,10 +649,10 @@
       <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="5">
         <v>48</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="5">
         <v>14</v>
       </c>
     </row>
@@ -674,10 +690,10 @@
       <c r="K4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="5">
         <v>0</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="5">
         <v>0</v>
       </c>
     </row>
@@ -715,10 +731,10 @@
       <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="5">
         <v>0</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="5">
         <v>0</v>
       </c>
     </row>
@@ -756,10 +772,10 @@
       <c r="K6" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="5">
         <v>0</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="5">
         <v>0</v>
       </c>
     </row>
@@ -797,10 +813,10 @@
       <c r="K7" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="5">
         <v>8</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="5">
         <v>3</v>
       </c>
     </row>
@@ -838,10 +854,10 @@
       <c r="K8" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="5">
         <v>6</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="5">
         <v>0</v>
       </c>
     </row>
@@ -879,10 +895,10 @@
       <c r="K9" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="5">
         <v>0</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="5">
         <v>0</v>
       </c>
     </row>
@@ -920,10 +936,10 @@
       <c r="K10" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="5">
         <v>0</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="5">
         <v>0</v>
       </c>
     </row>
@@ -961,10 +977,10 @@
       <c r="K11" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="3">
-        <v>15</v>
-      </c>
-      <c r="M11" s="3">
+      <c r="L11" s="5">
+        <v>15</v>
+      </c>
+      <c r="M11" s="5">
         <v>6</v>
       </c>
     </row>
@@ -1002,10 +1018,10 @@
       <c r="K12" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="5">
         <v>3</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1043,10 +1059,10 @@
       <c r="K13" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="5">
         <v>4</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1084,10 +1100,10 @@
       <c r="K14" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="5">
         <v>0</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1125,10 +1141,10 @@
       <c r="K15" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="5">
         <v>6</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="5">
         <v>3</v>
       </c>
     </row>
@@ -1166,10 +1182,10 @@
       <c r="K16" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="5">
         <v>1</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1207,10 +1223,10 @@
       <c r="K17" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17" s="5">
         <v>1</v>
       </c>
-      <c r="M17" s="3">
+      <c r="M17" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1248,10 +1264,10 @@
       <c r="K18" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="5">
         <v>9</v>
       </c>
-      <c r="M18" s="3">
+      <c r="M18" s="5">
         <v>3</v>
       </c>
     </row>
@@ -1289,10 +1305,10 @@
       <c r="K19" t="s">
         <v>18</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="5">
         <v>39</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M19" s="5">
         <v>16</v>
       </c>
     </row>
@@ -1330,10 +1346,10 @@
       <c r="K20" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="5">
         <v>3</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M20" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1371,10 +1387,10 @@
       <c r="K21" t="s">
         <v>18</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="5">
         <v>3</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1412,10 +1428,10 @@
       <c r="K22" t="s">
         <v>18</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22" s="5">
         <v>0</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1453,10 +1469,10 @@
       <c r="K23" t="s">
         <v>18</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23" s="5">
         <v>3</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1494,10 +1510,10 @@
       <c r="K24" t="s">
         <v>18</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24" s="5">
         <v>0</v>
       </c>
-      <c r="M24" s="3">
+      <c r="M24" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1535,10 +1551,10 @@
       <c r="K25" t="s">
         <v>18</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="5">
         <v>0</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M25" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1576,10 +1592,10 @@
       <c r="K26" t="s">
         <v>18</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26" s="5">
         <v>13</v>
       </c>
-      <c r="M26" s="3">
+      <c r="M26" s="5">
         <v>6</v>
       </c>
     </row>
@@ -1617,10 +1633,10 @@
       <c r="K27" t="s">
         <v>18</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="5">
         <v>27</v>
       </c>
-      <c r="M27" s="3">
+      <c r="M27" s="5">
         <v>8</v>
       </c>
     </row>
@@ -1658,10 +1674,10 @@
       <c r="K28" t="s">
         <v>18</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28" s="5">
         <v>3</v>
       </c>
-      <c r="M28" s="3">
+      <c r="M28" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1699,10 +1715,10 @@
       <c r="K29" t="s">
         <v>18</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29" s="5">
         <v>5</v>
       </c>
-      <c r="M29" s="3">
+      <c r="M29" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1740,10 +1756,10 @@
       <c r="K30" t="s">
         <v>18</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30" s="5">
         <v>5</v>
       </c>
-      <c r="M30" s="3">
+      <c r="M30" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1781,10 +1797,10 @@
       <c r="K31" t="s">
         <v>18</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="5">
         <v>1</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M31" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1822,10 +1838,10 @@
       <c r="K32" t="s">
         <v>18</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32" s="5">
         <v>9</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M32" s="5">
         <v>4</v>
       </c>
     </row>
@@ -1863,10 +1879,10 @@
       <c r="K33" t="s">
         <v>18</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33" s="5">
         <v>55</v>
       </c>
-      <c r="M33" s="3">
+      <c r="M33" s="5">
         <v>23</v>
       </c>
     </row>
@@ -1904,10 +1920,10 @@
       <c r="K34" t="s">
         <v>18</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34" s="5">
         <v>0</v>
       </c>
-      <c r="M34" s="3">
+      <c r="M34" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1945,10 +1961,10 @@
       <c r="K35" t="s">
         <v>18</v>
       </c>
-      <c r="L35" s="3">
+      <c r="L35" s="5">
         <v>14</v>
       </c>
-      <c r="M35" s="3">
+      <c r="M35" s="5">
         <v>5</v>
       </c>
     </row>
@@ -1986,10 +2002,10 @@
       <c r="K36" t="s">
         <v>18</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36" s="5">
         <v>4</v>
       </c>
-      <c r="M36" s="3">
+      <c r="M36" s="5">
         <v>1</v>
       </c>
     </row>
@@ -2027,10 +2043,10 @@
       <c r="K37" t="s">
         <v>18</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37" s="5">
         <v>0</v>
       </c>
-      <c r="M37" s="3">
+      <c r="M37" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2068,10 +2084,10 @@
       <c r="K38" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="5">
         <v>6</v>
       </c>
-      <c r="M38" s="3">
+      <c r="M38" s="5">
         <v>3</v>
       </c>
     </row>
@@ -2109,10 +2125,10 @@
       <c r="K39" t="s">
         <v>18</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L39" s="5">
         <v>4</v>
       </c>
-      <c r="M39" s="3">
+      <c r="M39" s="5">
         <v>2</v>
       </c>
     </row>
@@ -2150,10 +2166,10 @@
       <c r="K40" t="s">
         <v>18</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40" s="5">
         <v>3</v>
       </c>
-      <c r="M40" s="3">
+      <c r="M40" s="5">
         <v>1</v>
       </c>
     </row>
@@ -2191,10 +2207,10 @@
       <c r="K41" t="s">
         <v>18</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L41" s="5">
         <v>1</v>
       </c>
-      <c r="M41" s="3">
+      <c r="M41" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2232,10 +2248,10 @@
       <c r="K42" t="s">
         <v>18</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L42" s="5">
         <v>49</v>
       </c>
-      <c r="M42" s="3">
+      <c r="M42" s="5">
         <v>21</v>
       </c>
     </row>
@@ -2273,10 +2289,10 @@
       <c r="K43" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="3">
+      <c r="L43" s="5">
         <v>10</v>
       </c>
-      <c r="M43" s="3">
+      <c r="M43" s="5">
         <v>3</v>
       </c>
     </row>
@@ -2314,10 +2330,10 @@
       <c r="K44" t="s">
         <v>18</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L44" s="5">
         <v>2</v>
       </c>
-      <c r="M44" s="3">
+      <c r="M44" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2355,10 +2371,10 @@
       <c r="K45" t="s">
         <v>18</v>
       </c>
-      <c r="L45" s="3">
+      <c r="L45" s="5">
         <v>1</v>
       </c>
-      <c r="M45" s="3">
+      <c r="M45" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2396,10 +2412,10 @@
       <c r="K46" t="s">
         <v>18</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L46" s="5">
         <v>0</v>
       </c>
-      <c r="M46" s="3">
+      <c r="M46" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2437,10 +2453,10 @@
       <c r="K47" t="s">
         <v>18</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47" s="5">
         <v>4</v>
       </c>
-      <c r="M47" s="3">
+      <c r="M47" s="5">
         <v>2</v>
       </c>
     </row>
@@ -2478,10 +2494,10 @@
       <c r="K48" t="s">
         <v>18</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48" s="5">
         <v>0</v>
       </c>
-      <c r="M48" s="3">
+      <c r="M48" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2519,10 +2535,10 @@
       <c r="K49" t="s">
         <v>18</v>
       </c>
-      <c r="L49" s="3">
+      <c r="L49" s="5">
         <v>1</v>
       </c>
-      <c r="M49" s="3">
+      <c r="M49" s="5">
         <v>1</v>
       </c>
     </row>
@@ -2560,10 +2576,10 @@
       <c r="K50" t="s">
         <v>18</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50" s="5">
         <v>2</v>
       </c>
-      <c r="M50" s="3">
+      <c r="M50" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2601,10 +2617,10 @@
       <c r="K51" t="s">
         <v>18</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51" s="5">
         <v>45</v>
       </c>
-      <c r="M51" s="3">
+      <c r="M51" s="5">
         <v>18</v>
       </c>
     </row>
@@ -2642,10 +2658,10 @@
       <c r="K52" t="s">
         <v>18</v>
       </c>
-      <c r="L52" s="3">
+      <c r="L52" s="5">
         <v>9</v>
       </c>
-      <c r="M52" s="3">
+      <c r="M52" s="5">
         <v>2</v>
       </c>
     </row>
@@ -2683,10 +2699,10 @@
       <c r="K53" t="s">
         <v>18</v>
       </c>
-      <c r="L53" s="3">
+      <c r="L53" s="5">
         <v>12</v>
       </c>
-      <c r="M53" s="3">
+      <c r="M53" s="5">
         <v>2</v>
       </c>
     </row>
@@ -2724,10 +2740,10 @@
       <c r="K54" t="s">
         <v>18</v>
       </c>
-      <c r="L54" s="3">
+      <c r="L54" s="5">
         <v>0</v>
       </c>
-      <c r="M54" s="3">
+      <c r="M54" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2765,10 +2781,10 @@
       <c r="K55" t="s">
         <v>18</v>
       </c>
-      <c r="L55" s="3">
+      <c r="L55" s="5">
         <v>3</v>
       </c>
-      <c r="M55" s="3">
+      <c r="M55" s="5">
         <v>1</v>
       </c>
     </row>
@@ -2806,10 +2822,10 @@
       <c r="K56" t="s">
         <v>18</v>
       </c>
-      <c r="L56" s="3">
+      <c r="L56" s="5">
         <v>1</v>
       </c>
-      <c r="M56" s="3">
+      <c r="M56" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2847,10 +2863,10 @@
       <c r="K57" t="s">
         <v>18</v>
       </c>
-      <c r="L57" s="3">
+      <c r="L57" s="5">
         <v>0</v>
       </c>
-      <c r="M57" s="3">
+      <c r="M57" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2888,10 +2904,10 @@
       <c r="K58" t="s">
         <v>18</v>
       </c>
-      <c r="L58" s="3">
+      <c r="L58" s="5">
         <v>1</v>
       </c>
-      <c r="M58" s="3">
+      <c r="M58" s="5">
         <v>1</v>
       </c>
     </row>
@@ -2929,10 +2945,10 @@
       <c r="K59" t="s">
         <v>18</v>
       </c>
-      <c r="L59" s="3">
+      <c r="L59" s="5">
         <v>41</v>
       </c>
-      <c r="M59" s="3">
+      <c r="M59" s="5">
         <v>17</v>
       </c>
     </row>
@@ -2970,10 +2986,10 @@
       <c r="K60" t="s">
         <v>18</v>
       </c>
-      <c r="L60" s="3">
+      <c r="L60" s="5">
         <v>77</v>
       </c>
-      <c r="M60" s="3">
+      <c r="M60" s="5">
         <v>23</v>
       </c>
     </row>
@@ -3011,10 +3027,10 @@
       <c r="K61" t="s">
         <v>18</v>
       </c>
-      <c r="L61" s="3">
+      <c r="L61" s="5">
         <v>9</v>
       </c>
-      <c r="M61" s="3">
+      <c r="M61" s="5">
         <v>2</v>
       </c>
     </row>
@@ -3052,10 +3068,10 @@
       <c r="K62" t="s">
         <v>18</v>
       </c>
-      <c r="L62" s="3">
+      <c r="L62" s="5">
         <v>0</v>
       </c>
-      <c r="M62" s="3">
+      <c r="M62" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3093,10 +3109,10 @@
       <c r="K63" t="s">
         <v>18</v>
       </c>
-      <c r="L63" s="3">
+      <c r="L63" s="5">
         <v>3</v>
       </c>
-      <c r="M63" s="3">
+      <c r="M63" s="5">
         <v>1</v>
       </c>
     </row>
@@ -3134,10 +3150,10 @@
       <c r="K64" t="s">
         <v>18</v>
       </c>
-      <c r="L64" s="3">
+      <c r="L64" s="5">
         <v>6</v>
       </c>
-      <c r="M64" s="3">
+      <c r="M64" s="5">
         <v>3</v>
       </c>
     </row>
@@ -3175,10 +3191,10 @@
       <c r="K65" t="s">
         <v>18</v>
       </c>
-      <c r="L65" s="3">
+      <c r="L65" s="5">
         <v>16</v>
       </c>
-      <c r="M65" s="3">
+      <c r="M65" s="5">
         <v>4</v>
       </c>
     </row>
@@ -3216,10 +3232,10 @@
       <c r="K66" t="s">
         <v>18</v>
       </c>
-      <c r="L66" s="3">
+      <c r="L66" s="5">
         <v>37</v>
       </c>
-      <c r="M66" s="3">
+      <c r="M66" s="5">
         <v>16</v>
       </c>
     </row>
@@ -3257,10 +3273,10 @@
       <c r="K67" t="s">
         <v>18</v>
       </c>
-      <c r="L67" s="3">
+      <c r="L67" s="5">
         <v>9</v>
       </c>
-      <c r="M67" s="3">
+      <c r="M67" s="5">
         <v>2</v>
       </c>
     </row>
@@ -3298,10 +3314,10 @@
       <c r="K68" t="s">
         <v>18</v>
       </c>
-      <c r="L68" s="3">
-        <v>15</v>
-      </c>
-      <c r="M68" s="3">
+      <c r="L68" s="5">
+        <v>15</v>
+      </c>
+      <c r="M68" s="5">
         <v>3</v>
       </c>
     </row>
@@ -3339,10 +3355,10 @@
       <c r="K69" t="s">
         <v>18</v>
       </c>
-      <c r="L69" s="3">
+      <c r="L69" s="5">
         <v>2</v>
       </c>
-      <c r="M69" s="3">
+      <c r="M69" s="5">
         <v>1</v>
       </c>
     </row>
@@ -3380,10 +3396,10 @@
       <c r="K70" t="s">
         <v>18</v>
       </c>
-      <c r="L70" s="3">
+      <c r="L70" s="5">
         <v>0</v>
       </c>
-      <c r="M70" s="3">
+      <c r="M70" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3421,10 +3437,10 @@
       <c r="K71" t="s">
         <v>18</v>
       </c>
-      <c r="L71" s="3">
+      <c r="L71" s="5">
         <v>0</v>
       </c>
-      <c r="M71" s="3">
+      <c r="M71" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3462,10 +3478,10 @@
       <c r="K72" t="s">
         <v>18</v>
       </c>
-      <c r="L72" s="3">
+      <c r="L72" s="5">
         <v>41</v>
       </c>
-      <c r="M72" s="3">
+      <c r="M72" s="5">
         <v>4</v>
       </c>
     </row>
@@ -3503,10 +3519,10 @@
       <c r="K73" t="s">
         <v>18</v>
       </c>
-      <c r="L73" s="3">
+      <c r="L73" s="5">
         <v>4</v>
       </c>
-      <c r="M73" s="3">
+      <c r="M73" s="5">
         <v>2</v>
       </c>
     </row>
@@ -3544,10 +3560,10 @@
       <c r="K74" t="s">
         <v>18</v>
       </c>
-      <c r="L74" s="3">
+      <c r="L74" s="5">
         <v>31</v>
       </c>
-      <c r="M74" s="3">
+      <c r="M74" s="5">
         <v>13</v>
       </c>
     </row>
@@ -3585,10 +3601,10 @@
       <c r="K75" t="s">
         <v>18</v>
       </c>
-      <c r="L75" s="3">
+      <c r="L75" s="5">
         <v>33</v>
       </c>
-      <c r="M75" s="3">
+      <c r="M75" s="5">
         <v>10</v>
       </c>
     </row>
@@ -3626,10 +3642,10 @@
       <c r="K76" t="s">
         <v>18</v>
       </c>
-      <c r="L76" s="3">
+      <c r="L76" s="5">
         <v>7</v>
       </c>
-      <c r="M76" s="3">
+      <c r="M76" s="5">
         <v>2</v>
       </c>
     </row>
@@ -3667,10 +3683,10 @@
       <c r="K77" t="s">
         <v>18</v>
       </c>
-      <c r="L77" s="3">
+      <c r="L77" s="5">
         <v>16</v>
       </c>
-      <c r="M77" s="3">
+      <c r="M77" s="5">
         <v>6</v>
       </c>
     </row>
@@ -3708,10 +3724,10 @@
       <c r="K78" t="s">
         <v>18</v>
       </c>
-      <c r="L78" s="3">
+      <c r="L78" s="5">
         <v>0</v>
       </c>
-      <c r="M78" s="3">
+      <c r="M78" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3749,10 +3765,10 @@
       <c r="K79" t="s">
         <v>18</v>
       </c>
-      <c r="L79" s="3">
+      <c r="L79" s="5">
         <v>1</v>
       </c>
-      <c r="M79" s="3">
+      <c r="M79" s="5">
         <v>1</v>
       </c>
     </row>
@@ -3790,10 +3806,10 @@
       <c r="K80" t="s">
         <v>18</v>
       </c>
-      <c r="L80" s="3">
+      <c r="L80" s="5">
         <v>8</v>
       </c>
-      <c r="M80" s="3">
+      <c r="M80" s="5">
         <v>4</v>
       </c>
     </row>
@@ -3831,10 +3847,10 @@
       <c r="K81" t="s">
         <v>18</v>
       </c>
-      <c r="L81" s="3">
+      <c r="L81" s="5">
         <v>2</v>
       </c>
-      <c r="M81" s="3">
+      <c r="M81" s="5">
         <v>1</v>
       </c>
     </row>
@@ -3872,10 +3888,10 @@
       <c r="K82" t="s">
         <v>18</v>
       </c>
-      <c r="L82" s="3">
+      <c r="L82" s="5">
         <v>1</v>
       </c>
-      <c r="M82" s="3">
+      <c r="M82" s="5">
         <v>0</v>
       </c>
     </row>
@@ -3913,10 +3929,10 @@
       <c r="K83" t="s">
         <v>18</v>
       </c>
-      <c r="L83" s="3">
-        <v>17</v>
-      </c>
-      <c r="M83" s="3">
+      <c r="L83" s="5">
+        <v>17</v>
+      </c>
+      <c r="M83" s="5">
         <v>7</v>
       </c>
     </row>
@@ -3954,10 +3970,10 @@
       <c r="K84" t="s">
         <v>18</v>
       </c>
-      <c r="L84" s="3">
+      <c r="L84" s="5">
         <v>6</v>
       </c>
-      <c r="M84" s="3">
+      <c r="M84" s="5">
         <v>2</v>
       </c>
     </row>
@@ -3995,10 +4011,10 @@
       <c r="K85" t="s">
         <v>18</v>
       </c>
-      <c r="L85" s="3">
+      <c r="L85" s="5">
         <v>2</v>
       </c>
-      <c r="M85" s="3">
+      <c r="M85" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4036,10 +4052,10 @@
       <c r="K86" t="s">
         <v>18</v>
       </c>
-      <c r="L86" s="3">
+      <c r="L86" s="5">
         <v>7</v>
       </c>
-      <c r="M86" s="3">
+      <c r="M86" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4077,10 +4093,10 @@
       <c r="K87" t="s">
         <v>18</v>
       </c>
-      <c r="L87" s="3">
+      <c r="L87" s="5">
         <v>1</v>
       </c>
-      <c r="M87" s="3">
+      <c r="M87" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4118,10 +4134,10 @@
       <c r="K88" t="s">
         <v>18</v>
       </c>
-      <c r="L88" s="3">
+      <c r="L88" s="5">
         <v>6</v>
       </c>
-      <c r="M88" s="3">
+      <c r="M88" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4159,10 +4175,10 @@
       <c r="K89" t="s">
         <v>18</v>
       </c>
-      <c r="L89" s="3">
+      <c r="L89" s="5">
         <v>8</v>
       </c>
-      <c r="M89" s="3">
+      <c r="M89" s="5">
         <v>4</v>
       </c>
     </row>
@@ -4200,10 +4216,10 @@
       <c r="K90" t="s">
         <v>18</v>
       </c>
-      <c r="L90" s="3">
+      <c r="L90" s="5">
         <v>11</v>
       </c>
-      <c r="M90" s="3">
+      <c r="M90" s="5">
         <v>4</v>
       </c>
     </row>
@@ -4241,10 +4257,10 @@
       <c r="K91" t="s">
         <v>18</v>
       </c>
-      <c r="L91" s="3">
+      <c r="L91" s="5">
         <v>0</v>
       </c>
-      <c r="M91" s="3">
+      <c r="M91" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4282,10 +4298,10 @@
       <c r="K92" t="s">
         <v>18</v>
       </c>
-      <c r="L92" s="3">
+      <c r="L92" s="5">
         <v>6</v>
       </c>
-      <c r="M92" s="3">
+      <c r="M92" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4323,10 +4339,10 @@
       <c r="K93" t="s">
         <v>18</v>
       </c>
-      <c r="L93" s="3">
+      <c r="L93" s="5">
         <v>20</v>
       </c>
-      <c r="M93" s="3">
+      <c r="M93" s="5">
         <v>9</v>
       </c>
     </row>
@@ -4364,10 +4380,10 @@
       <c r="K94" t="s">
         <v>18</v>
       </c>
-      <c r="L94" s="3">
-        <v>15</v>
-      </c>
-      <c r="M94" s="3">
+      <c r="L94" s="5">
+        <v>15</v>
+      </c>
+      <c r="M94" s="5">
         <v>6</v>
       </c>
     </row>
@@ -4405,10 +4421,10 @@
       <c r="K95" t="s">
         <v>18</v>
       </c>
-      <c r="L95" s="3">
+      <c r="L95" s="5">
         <v>4</v>
       </c>
-      <c r="M95" s="3">
+      <c r="M95" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4446,10 +4462,10 @@
       <c r="K96" t="s">
         <v>18</v>
       </c>
-      <c r="L96" s="3">
+      <c r="L96" s="5">
         <v>0</v>
       </c>
-      <c r="M96" s="3">
+      <c r="M96" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4487,10 +4503,10 @@
       <c r="K97" t="s">
         <v>18</v>
       </c>
-      <c r="L97" s="3">
+      <c r="L97" s="5">
         <v>8</v>
       </c>
-      <c r="M97" s="3">
+      <c r="M97" s="5">
         <v>4</v>
       </c>
     </row>
@@ -4528,10 +4544,10 @@
       <c r="K98" t="s">
         <v>18</v>
       </c>
-      <c r="L98" s="3">
+      <c r="L98" s="5">
         <v>4</v>
       </c>
-      <c r="M98" s="3">
+      <c r="M98" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4569,10 +4585,10 @@
       <c r="K99" t="s">
         <v>18</v>
       </c>
-      <c r="L99" s="3">
+      <c r="L99" s="5">
         <v>4</v>
       </c>
-      <c r="M99" s="3">
+      <c r="M99" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4610,10 +4626,10 @@
       <c r="K100" t="s">
         <v>18</v>
       </c>
-      <c r="L100" s="3">
+      <c r="L100" s="5">
         <v>1</v>
       </c>
-      <c r="M100" s="3">
+      <c r="M100" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4651,10 +4667,10 @@
       <c r="K101" t="s">
         <v>18</v>
       </c>
-      <c r="L101" s="3">
+      <c r="L101" s="5">
         <v>13</v>
       </c>
-      <c r="M101" s="3">
+      <c r="M101" s="5">
         <v>5</v>
       </c>
     </row>
@@ -4692,10 +4708,10 @@
       <c r="K102" t="s">
         <v>18</v>
       </c>
-      <c r="L102" s="3">
+      <c r="L102" s="5">
         <v>28</v>
       </c>
-      <c r="M102" s="3">
+      <c r="M102" s="5">
         <v>9</v>
       </c>
     </row>
@@ -4733,10 +4749,10 @@
       <c r="K103" t="s">
         <v>18</v>
       </c>
-      <c r="L103" s="3">
+      <c r="L103" s="5">
         <v>1</v>
       </c>
-      <c r="M103" s="3">
+      <c r="M103" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4746,8 +4762,6 @@
       <c r="C104" s="3"/>
       <c r="F104" s="3"/>
       <c r="J104" s="3"/>
-      <c r="L104" s="3"/>
-      <c r="M104" s="3"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
@@ -4755,8 +4769,6 @@
       <c r="C105" s="3"/>
       <c r="F105" s="3"/>
       <c r="J105" s="3"/>
-      <c r="L105" s="3"/>
-      <c r="M105" s="3"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
@@ -4764,8 +4776,6 @@
       <c r="C106" s="3"/>
       <c r="F106" s="3"/>
       <c r="J106" s="3"/>
-      <c r="L106" s="3"/>
-      <c r="M106" s="3"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
@@ -4773,8 +4783,6 @@
       <c r="C107" s="3"/>
       <c r="F107" s="3"/>
       <c r="J107" s="3"/>
-      <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
@@ -4782,8 +4790,6 @@
       <c r="C108" s="3"/>
       <c r="F108" s="3"/>
       <c r="J108" s="3"/>
-      <c r="L108" s="3"/>
-      <c r="M108" s="3"/>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
@@ -4791,8 +4797,6 @@
       <c r="C109" s="3"/>
       <c r="F109" s="3"/>
       <c r="J109" s="3"/>
-      <c r="L109" s="3"/>
-      <c r="M109" s="3"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
@@ -4800,8 +4804,6 @@
       <c r="C110" s="3"/>
       <c r="F110" s="3"/>
       <c r="J110" s="3"/>
-      <c r="L110" s="3"/>
-      <c r="M110" s="3"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
@@ -4809,8 +4811,6 @@
       <c r="C111" s="3"/>
       <c r="F111" s="3"/>
       <c r="J111" s="3"/>
-      <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
@@ -4818,2108 +4818,1641 @@
       <c r="C112" s="3"/>
       <c r="F112" s="3"/>
       <c r="J112" s="3"/>
-      <c r="L112" s="3"/>
-      <c r="M112" s="3"/>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="3"/>
       <c r="F113" s="3"/>
       <c r="J113" s="3"/>
-      <c r="L113" s="3"/>
-      <c r="M113" s="3"/>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="3"/>
       <c r="F114" s="3"/>
       <c r="J114" s="3"/>
-      <c r="L114" s="3"/>
-      <c r="M114" s="3"/>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="3"/>
       <c r="F115" s="3"/>
       <c r="J115" s="3"/>
-      <c r="L115" s="3"/>
-      <c r="M115" s="3"/>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="3"/>
       <c r="F116" s="3"/>
       <c r="J116" s="3"/>
-      <c r="L116" s="3"/>
-      <c r="M116" s="3"/>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="3"/>
       <c r="F117" s="3"/>
       <c r="J117" s="3"/>
-      <c r="L117" s="3"/>
-      <c r="M117" s="3"/>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="3"/>
       <c r="F118" s="3"/>
       <c r="J118" s="3"/>
-      <c r="L118" s="3"/>
-      <c r="M118" s="3"/>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="3"/>
       <c r="F119" s="3"/>
       <c r="J119" s="3"/>
-      <c r="L119" s="3"/>
-      <c r="M119" s="3"/>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="3"/>
       <c r="F120" s="3"/>
       <c r="J120" s="3"/>
-      <c r="L120" s="3"/>
-      <c r="M120" s="3"/>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="3"/>
       <c r="F121" s="3"/>
       <c r="J121" s="3"/>
-      <c r="L121" s="3"/>
-      <c r="M121" s="3"/>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="3"/>
       <c r="F122" s="3"/>
       <c r="J122" s="3"/>
-      <c r="L122" s="3"/>
-      <c r="M122" s="3"/>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="3"/>
       <c r="F123" s="3"/>
       <c r="J123" s="3"/>
-      <c r="L123" s="3"/>
-      <c r="M123" s="3"/>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="3"/>
       <c r="F124" s="3"/>
       <c r="J124" s="3"/>
-      <c r="L124" s="3"/>
-      <c r="M124" s="3"/>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="3"/>
       <c r="F125" s="3"/>
       <c r="J125" s="3"/>
-      <c r="L125" s="3"/>
-      <c r="M125" s="3"/>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="3"/>
       <c r="F126" s="3"/>
       <c r="J126" s="3"/>
-      <c r="L126" s="3"/>
-      <c r="M126" s="3"/>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="3"/>
       <c r="F127" s="3"/>
       <c r="J127" s="3"/>
-      <c r="L127" s="3"/>
-      <c r="M127" s="3"/>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="3"/>
       <c r="F128" s="3"/>
       <c r="J128" s="3"/>
-      <c r="L128" s="3"/>
-      <c r="M128" s="3"/>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="3"/>
       <c r="F129" s="3"/>
       <c r="J129" s="3"/>
-      <c r="L129" s="3"/>
-      <c r="M129" s="3"/>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="3"/>
       <c r="F130" s="3"/>
       <c r="J130" s="3"/>
-      <c r="L130" s="3"/>
-      <c r="M130" s="3"/>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="3"/>
       <c r="F131" s="3"/>
       <c r="J131" s="3"/>
-      <c r="L131" s="3"/>
-      <c r="M131" s="3"/>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="3"/>
       <c r="F132" s="3"/>
       <c r="J132" s="3"/>
-      <c r="L132" s="3"/>
-      <c r="M132" s="3"/>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="3"/>
       <c r="F133" s="3"/>
       <c r="J133" s="3"/>
-      <c r="L133" s="3"/>
-      <c r="M133" s="3"/>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="3"/>
       <c r="F134" s="3"/>
       <c r="J134" s="3"/>
-      <c r="L134" s="3"/>
-      <c r="M134" s="3"/>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="3"/>
       <c r="F135" s="3"/>
       <c r="J135" s="3"/>
-      <c r="L135" s="3"/>
-      <c r="M135" s="3"/>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="3"/>
       <c r="F136" s="3"/>
       <c r="J136" s="3"/>
-      <c r="L136" s="3"/>
-      <c r="M136" s="3"/>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="3"/>
       <c r="F137" s="3"/>
       <c r="J137" s="3"/>
-      <c r="L137" s="3"/>
-      <c r="M137" s="3"/>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="3"/>
       <c r="F138" s="3"/>
       <c r="J138" s="3"/>
-      <c r="L138" s="3"/>
-      <c r="M138" s="3"/>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="3"/>
       <c r="F139" s="3"/>
       <c r="J139" s="3"/>
-      <c r="L139" s="3"/>
-      <c r="M139" s="3"/>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="3"/>
       <c r="F140" s="3"/>
       <c r="J140" s="3"/>
-      <c r="L140" s="3"/>
-      <c r="M140" s="3"/>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="3"/>
       <c r="F141" s="3"/>
       <c r="J141" s="3"/>
-      <c r="L141" s="3"/>
-      <c r="M141" s="3"/>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="3"/>
       <c r="F142" s="3"/>
       <c r="J142" s="3"/>
-      <c r="L142" s="3"/>
-      <c r="M142" s="3"/>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="3"/>
       <c r="F143" s="3"/>
       <c r="J143" s="3"/>
-      <c r="L143" s="3"/>
-      <c r="M143" s="3"/>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="3"/>
       <c r="F144" s="3"/>
       <c r="J144" s="3"/>
-      <c r="L144" s="3"/>
-      <c r="M144" s="3"/>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="3"/>
       <c r="F145" s="3"/>
       <c r="J145" s="3"/>
-      <c r="L145" s="3"/>
-      <c r="M145" s="3"/>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="3"/>
       <c r="F146" s="3"/>
       <c r="J146" s="3"/>
-      <c r="L146" s="3"/>
-      <c r="M146" s="3"/>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="3"/>
       <c r="F147" s="3"/>
       <c r="J147" s="3"/>
-      <c r="L147" s="3"/>
-      <c r="M147" s="3"/>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="3"/>
       <c r="F148" s="3"/>
       <c r="J148" s="3"/>
-      <c r="L148" s="3"/>
-      <c r="M148" s="3"/>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="3"/>
       <c r="F149" s="3"/>
       <c r="J149" s="3"/>
-      <c r="L149" s="3"/>
-      <c r="M149" s="3"/>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="3"/>
       <c r="F150" s="3"/>
       <c r="J150" s="3"/>
-      <c r="L150" s="3"/>
-      <c r="M150" s="3"/>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="3"/>
       <c r="F151" s="3"/>
       <c r="J151" s="3"/>
-      <c r="L151" s="3"/>
-      <c r="M151" s="3"/>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="3"/>
       <c r="F152" s="3"/>
       <c r="J152" s="3"/>
-      <c r="L152" s="3"/>
-      <c r="M152" s="3"/>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="3"/>
       <c r="F153" s="3"/>
       <c r="J153" s="3"/>
-      <c r="L153" s="3"/>
-      <c r="M153" s="3"/>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="3"/>
       <c r="F154" s="3"/>
       <c r="J154" s="3"/>
-      <c r="L154" s="3"/>
-      <c r="M154" s="3"/>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="3"/>
       <c r="F155" s="3"/>
       <c r="J155" s="3"/>
-      <c r="L155" s="3"/>
-      <c r="M155" s="3"/>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="3"/>
       <c r="F156" s="3"/>
       <c r="J156" s="3"/>
-      <c r="L156" s="3"/>
-      <c r="M156" s="3"/>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="3"/>
       <c r="F157" s="3"/>
       <c r="J157" s="3"/>
-      <c r="L157" s="3"/>
-      <c r="M157" s="3"/>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="3"/>
       <c r="F158" s="3"/>
       <c r="J158" s="3"/>
-      <c r="L158" s="3"/>
-      <c r="M158" s="3"/>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="3"/>
       <c r="F159" s="3"/>
       <c r="J159" s="3"/>
-      <c r="L159" s="3"/>
-      <c r="M159" s="3"/>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="3"/>
       <c r="F160" s="3"/>
       <c r="J160" s="3"/>
-      <c r="L160" s="3"/>
-      <c r="M160" s="3"/>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="3"/>
       <c r="F161" s="3"/>
       <c r="J161" s="3"/>
-      <c r="L161" s="3"/>
-      <c r="M161" s="3"/>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="3"/>
       <c r="F162" s="3"/>
       <c r="J162" s="3"/>
-      <c r="L162" s="3"/>
-      <c r="M162" s="3"/>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="3"/>
       <c r="F163" s="3"/>
       <c r="J163" s="3"/>
-      <c r="L163" s="3"/>
-      <c r="M163" s="3"/>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="3"/>
       <c r="F164" s="3"/>
       <c r="J164" s="3"/>
-      <c r="L164" s="3"/>
-      <c r="M164" s="3"/>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="3"/>
       <c r="F165" s="3"/>
       <c r="J165" s="3"/>
-      <c r="L165" s="3"/>
-      <c r="M165" s="3"/>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="3"/>
       <c r="F166" s="3"/>
       <c r="J166" s="3"/>
-      <c r="L166" s="3"/>
-      <c r="M166" s="3"/>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="3"/>
       <c r="F167" s="3"/>
       <c r="J167" s="3"/>
-      <c r="L167" s="3"/>
-      <c r="M167" s="3"/>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="3"/>
       <c r="F168" s="3"/>
       <c r="J168" s="3"/>
-      <c r="L168" s="3"/>
-      <c r="M168" s="3"/>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="3"/>
       <c r="F169" s="3"/>
       <c r="J169" s="3"/>
-      <c r="L169" s="3"/>
-      <c r="M169" s="3"/>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="3"/>
       <c r="F170" s="3"/>
       <c r="J170" s="3"/>
-      <c r="L170" s="3"/>
-      <c r="M170" s="3"/>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="3"/>
       <c r="F171" s="3"/>
       <c r="J171" s="3"/>
-      <c r="L171" s="3"/>
-      <c r="M171" s="3"/>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="3"/>
       <c r="F172" s="3"/>
       <c r="J172" s="3"/>
-      <c r="L172" s="3"/>
-      <c r="M172" s="3"/>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="3"/>
       <c r="F173" s="3"/>
       <c r="J173" s="3"/>
-      <c r="L173" s="3"/>
-      <c r="M173" s="3"/>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="3"/>
       <c r="F174" s="3"/>
       <c r="J174" s="3"/>
-      <c r="L174" s="3"/>
-      <c r="M174" s="3"/>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="3"/>
       <c r="F175" s="3"/>
       <c r="J175" s="3"/>
-      <c r="L175" s="3"/>
-      <c r="M175" s="3"/>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="3"/>
       <c r="F176" s="3"/>
       <c r="J176" s="3"/>
-      <c r="L176" s="3"/>
-      <c r="M176" s="3"/>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="3"/>
       <c r="F177" s="3"/>
       <c r="J177" s="3"/>
-      <c r="L177" s="3"/>
-      <c r="M177" s="3"/>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="3"/>
       <c r="F178" s="3"/>
       <c r="J178" s="3"/>
-      <c r="L178" s="3"/>
-      <c r="M178" s="3"/>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="3"/>
       <c r="F179" s="3"/>
       <c r="J179" s="3"/>
-      <c r="L179" s="3"/>
-      <c r="M179" s="3"/>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="3"/>
       <c r="F180" s="3"/>
       <c r="J180" s="3"/>
-      <c r="L180" s="3"/>
-      <c r="M180" s="3"/>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="3"/>
       <c r="F181" s="3"/>
       <c r="J181" s="3"/>
-      <c r="L181" s="3"/>
-      <c r="M181" s="3"/>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="3"/>
       <c r="F182" s="3"/>
       <c r="J182" s="3"/>
-      <c r="L182" s="3"/>
-      <c r="M182" s="3"/>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="3"/>
       <c r="F183" s="3"/>
       <c r="J183" s="3"/>
-      <c r="L183" s="3"/>
-      <c r="M183" s="3"/>
-    </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="3"/>
       <c r="F184" s="3"/>
       <c r="J184" s="3"/>
-      <c r="L184" s="3"/>
-      <c r="M184" s="3"/>
-    </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="3"/>
       <c r="F185" s="3"/>
       <c r="J185" s="3"/>
-      <c r="L185" s="3"/>
-      <c r="M185" s="3"/>
-    </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="3"/>
       <c r="F186" s="3"/>
       <c r="J186" s="3"/>
-      <c r="L186" s="3"/>
-      <c r="M186" s="3"/>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="3"/>
       <c r="F187" s="3"/>
       <c r="J187" s="3"/>
-      <c r="L187" s="3"/>
-      <c r="M187" s="3"/>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="3"/>
       <c r="F188" s="3"/>
       <c r="J188" s="3"/>
-      <c r="L188" s="3"/>
-      <c r="M188" s="3"/>
-    </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="3"/>
       <c r="F189" s="3"/>
       <c r="J189" s="3"/>
-      <c r="L189" s="3"/>
-      <c r="M189" s="3"/>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="3"/>
       <c r="F190" s="3"/>
       <c r="J190" s="3"/>
-      <c r="L190" s="3"/>
-      <c r="M190" s="3"/>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="3"/>
       <c r="F191" s="3"/>
       <c r="J191" s="3"/>
-      <c r="L191" s="3"/>
-      <c r="M191" s="3"/>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="3"/>
       <c r="F192" s="3"/>
       <c r="J192" s="3"/>
-      <c r="L192" s="3"/>
-      <c r="M192" s="3"/>
-    </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="3"/>
       <c r="F193" s="3"/>
       <c r="J193" s="3"/>
-      <c r="L193" s="3"/>
-      <c r="M193" s="3"/>
-    </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="3"/>
       <c r="F194" s="3"/>
       <c r="J194" s="3"/>
-      <c r="L194" s="3"/>
-      <c r="M194" s="3"/>
-    </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="3"/>
       <c r="F195" s="3"/>
       <c r="J195" s="3"/>
-      <c r="L195" s="3"/>
-      <c r="M195" s="3"/>
-    </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="3"/>
       <c r="F196" s="3"/>
       <c r="J196" s="3"/>
-      <c r="L196" s="3"/>
-      <c r="M196" s="3"/>
-    </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="3"/>
       <c r="F197" s="3"/>
       <c r="J197" s="3"/>
-      <c r="L197" s="3"/>
-      <c r="M197" s="3"/>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="3"/>
       <c r="F198" s="3"/>
       <c r="J198" s="3"/>
-      <c r="L198" s="3"/>
-      <c r="M198" s="3"/>
-    </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="3"/>
       <c r="F199" s="3"/>
       <c r="J199" s="3"/>
-      <c r="L199" s="3"/>
-      <c r="M199" s="3"/>
-    </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="3"/>
       <c r="F200" s="3"/>
       <c r="J200" s="3"/>
-      <c r="L200" s="3"/>
-      <c r="M200" s="3"/>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="3"/>
       <c r="F201" s="3"/>
       <c r="J201" s="3"/>
-      <c r="L201" s="3"/>
-      <c r="M201" s="3"/>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="3"/>
       <c r="F202" s="3"/>
       <c r="J202" s="3"/>
-      <c r="L202" s="3"/>
-      <c r="M202" s="3"/>
-    </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="3"/>
       <c r="F203" s="3"/>
       <c r="J203" s="3"/>
-      <c r="L203" s="3"/>
-      <c r="M203" s="3"/>
-    </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
       <c r="C204" s="3"/>
       <c r="F204" s="3"/>
       <c r="J204" s="3"/>
-      <c r="L204" s="3"/>
-      <c r="M204" s="3"/>
-    </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
       <c r="C205" s="3"/>
       <c r="F205" s="3"/>
       <c r="J205" s="3"/>
-      <c r="L205" s="3"/>
-      <c r="M205" s="3"/>
-    </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="3"/>
       <c r="F206" s="3"/>
       <c r="J206" s="3"/>
-      <c r="L206" s="3"/>
-      <c r="M206" s="3"/>
-    </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="3"/>
       <c r="F207" s="3"/>
       <c r="J207" s="3"/>
-      <c r="L207" s="3"/>
-      <c r="M207" s="3"/>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="3"/>
       <c r="F208" s="3"/>
       <c r="J208" s="3"/>
-      <c r="L208" s="3"/>
-      <c r="M208" s="3"/>
-    </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="3"/>
       <c r="F209" s="3"/>
       <c r="J209" s="3"/>
-      <c r="L209" s="3"/>
-      <c r="M209" s="3"/>
-    </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="3"/>
       <c r="F210" s="3"/>
       <c r="J210" s="3"/>
-      <c r="L210" s="3"/>
-      <c r="M210" s="3"/>
-    </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="3"/>
       <c r="F211" s="3"/>
       <c r="J211" s="3"/>
-      <c r="L211" s="3"/>
-      <c r="M211" s="3"/>
-    </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="3"/>
       <c r="F212" s="3"/>
       <c r="J212" s="3"/>
-      <c r="L212" s="3"/>
-      <c r="M212" s="3"/>
-    </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="3"/>
       <c r="F213" s="3"/>
       <c r="J213" s="3"/>
-      <c r="L213" s="3"/>
-      <c r="M213" s="3"/>
-    </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="3"/>
       <c r="F214" s="3"/>
       <c r="J214" s="3"/>
-      <c r="L214" s="3"/>
-      <c r="M214" s="3"/>
-    </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="3"/>
       <c r="F215" s="3"/>
       <c r="J215" s="3"/>
-      <c r="L215" s="3"/>
-      <c r="M215" s="3"/>
-    </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="3"/>
       <c r="F216" s="3"/>
       <c r="J216" s="3"/>
-      <c r="L216" s="3"/>
-      <c r="M216" s="3"/>
-    </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
       <c r="C217" s="3"/>
       <c r="F217" s="3"/>
       <c r="J217" s="3"/>
-      <c r="L217" s="3"/>
-      <c r="M217" s="3"/>
-    </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="3"/>
       <c r="F218" s="3"/>
       <c r="J218" s="3"/>
-      <c r="L218" s="3"/>
-      <c r="M218" s="3"/>
-    </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
       <c r="C219" s="3"/>
       <c r="F219" s="3"/>
       <c r="J219" s="3"/>
-      <c r="L219" s="3"/>
-      <c r="M219" s="3"/>
-    </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="3"/>
       <c r="F220" s="3"/>
       <c r="J220" s="3"/>
-      <c r="L220" s="3"/>
-      <c r="M220" s="3"/>
-    </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
       <c r="C221" s="3"/>
       <c r="F221" s="3"/>
       <c r="J221" s="3"/>
-      <c r="L221" s="3"/>
-      <c r="M221" s="3"/>
-    </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
       <c r="C222" s="3"/>
       <c r="F222" s="3"/>
       <c r="J222" s="3"/>
-      <c r="L222" s="3"/>
-      <c r="M222" s="3"/>
-    </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
       <c r="C223" s="3"/>
       <c r="F223" s="3"/>
       <c r="J223" s="3"/>
-      <c r="L223" s="3"/>
-      <c r="M223" s="3"/>
-    </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
       <c r="C224" s="3"/>
       <c r="F224" s="3"/>
       <c r="J224" s="3"/>
-      <c r="L224" s="3"/>
-      <c r="M224" s="3"/>
-    </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
       <c r="C225" s="3"/>
       <c r="F225" s="3"/>
       <c r="J225" s="3"/>
-      <c r="L225" s="3"/>
-      <c r="M225" s="3"/>
-    </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
       <c r="C226" s="3"/>
       <c r="F226" s="3"/>
       <c r="J226" s="3"/>
-      <c r="L226" s="3"/>
-      <c r="M226" s="3"/>
-    </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="3"/>
       <c r="F227" s="3"/>
       <c r="J227" s="3"/>
-      <c r="L227" s="3"/>
-      <c r="M227" s="3"/>
-    </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
       <c r="C228" s="3"/>
       <c r="F228" s="3"/>
       <c r="J228" s="3"/>
-      <c r="L228" s="3"/>
-      <c r="M228" s="3"/>
-    </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="2"/>
       <c r="C229" s="3"/>
       <c r="F229" s="3"/>
       <c r="J229" s="3"/>
-      <c r="L229" s="3"/>
-      <c r="M229" s="3"/>
-    </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
       <c r="C230" s="3"/>
       <c r="F230" s="3"/>
       <c r="J230" s="3"/>
-      <c r="L230" s="3"/>
-      <c r="M230" s="3"/>
-    </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
       <c r="C231" s="3"/>
       <c r="F231" s="3"/>
       <c r="J231" s="3"/>
-      <c r="L231" s="3"/>
-      <c r="M231" s="3"/>
-    </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
       <c r="C232" s="3"/>
       <c r="F232" s="3"/>
       <c r="J232" s="3"/>
-      <c r="L232" s="3"/>
-      <c r="M232" s="3"/>
-    </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
       <c r="B233" s="2"/>
       <c r="C233" s="3"/>
       <c r="F233" s="3"/>
       <c r="J233" s="3"/>
-      <c r="L233" s="3"/>
-      <c r="M233" s="3"/>
-    </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
       <c r="B234" s="2"/>
       <c r="C234" s="3"/>
       <c r="F234" s="3"/>
       <c r="J234" s="3"/>
-      <c r="L234" s="3"/>
-      <c r="M234" s="3"/>
-    </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
       <c r="B235" s="2"/>
       <c r="C235" s="3"/>
       <c r="F235" s="3"/>
       <c r="J235" s="3"/>
-      <c r="L235" s="3"/>
-      <c r="M235" s="3"/>
-    </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
       <c r="B236" s="2"/>
       <c r="C236" s="3"/>
       <c r="F236" s="3"/>
       <c r="J236" s="3"/>
-      <c r="L236" s="3"/>
-      <c r="M236" s="3"/>
-    </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
       <c r="B237" s="2"/>
       <c r="C237" s="3"/>
       <c r="F237" s="3"/>
       <c r="J237" s="3"/>
-      <c r="L237" s="3"/>
-      <c r="M237" s="3"/>
-    </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
       <c r="B238" s="2"/>
       <c r="C238" s="3"/>
       <c r="F238" s="3"/>
       <c r="J238" s="3"/>
-      <c r="L238" s="3"/>
-      <c r="M238" s="3"/>
-    </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
       <c r="B239" s="2"/>
       <c r="C239" s="3"/>
       <c r="F239" s="3"/>
       <c r="J239" s="3"/>
-      <c r="L239" s="3"/>
-      <c r="M239" s="3"/>
-    </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
       <c r="B240" s="2"/>
       <c r="C240" s="3"/>
       <c r="F240" s="3"/>
       <c r="J240" s="3"/>
-      <c r="L240" s="3"/>
-      <c r="M240" s="3"/>
-    </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
       <c r="B241" s="2"/>
       <c r="C241" s="3"/>
       <c r="F241" s="3"/>
       <c r="J241" s="3"/>
-      <c r="L241" s="3"/>
-      <c r="M241" s="3"/>
-    </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
       <c r="B242" s="2"/>
       <c r="C242" s="3"/>
       <c r="F242" s="3"/>
       <c r="J242" s="3"/>
-      <c r="L242" s="3"/>
-      <c r="M242" s="3"/>
-    </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
       <c r="B243" s="2"/>
       <c r="C243" s="3"/>
       <c r="F243" s="3"/>
       <c r="J243" s="3"/>
-      <c r="L243" s="3"/>
-      <c r="M243" s="3"/>
-    </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
       <c r="B244" s="2"/>
       <c r="C244" s="3"/>
       <c r="F244" s="3"/>
       <c r="J244" s="3"/>
-      <c r="L244" s="3"/>
-      <c r="M244" s="3"/>
-    </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="2"/>
       <c r="B245" s="2"/>
       <c r="C245" s="3"/>
       <c r="F245" s="3"/>
       <c r="J245" s="3"/>
-      <c r="L245" s="3"/>
-      <c r="M245" s="3"/>
-    </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
       <c r="B246" s="2"/>
       <c r="C246" s="3"/>
       <c r="F246" s="3"/>
       <c r="J246" s="3"/>
-      <c r="L246" s="3"/>
-      <c r="M246" s="3"/>
-    </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
       <c r="C247" s="3"/>
       <c r="F247" s="3"/>
       <c r="J247" s="3"/>
-      <c r="L247" s="3"/>
-      <c r="M247" s="3"/>
-    </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
       <c r="B248" s="2"/>
       <c r="C248" s="3"/>
       <c r="F248" s="3"/>
       <c r="J248" s="3"/>
-      <c r="L248" s="3"/>
-      <c r="M248" s="3"/>
-    </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
       <c r="B249" s="2"/>
       <c r="C249" s="3"/>
       <c r="F249" s="3"/>
       <c r="J249" s="3"/>
-      <c r="L249" s="3"/>
-      <c r="M249" s="3"/>
-    </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="2"/>
       <c r="B250" s="2"/>
       <c r="C250" s="3"/>
       <c r="F250" s="3"/>
       <c r="J250" s="3"/>
-      <c r="L250" s="3"/>
-      <c r="M250" s="3"/>
-    </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
       <c r="C251" s="3"/>
       <c r="F251" s="3"/>
       <c r="J251" s="3"/>
-      <c r="L251" s="3"/>
-      <c r="M251" s="3"/>
-    </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="2"/>
       <c r="B252" s="2"/>
       <c r="C252" s="3"/>
       <c r="F252" s="3"/>
       <c r="J252" s="3"/>
-      <c r="L252" s="3"/>
-      <c r="M252" s="3"/>
-    </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="2"/>
       <c r="B253" s="2"/>
       <c r="C253" s="3"/>
       <c r="F253" s="3"/>
       <c r="J253" s="3"/>
-      <c r="L253" s="3"/>
-      <c r="M253" s="3"/>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="2"/>
       <c r="B254" s="2"/>
       <c r="C254" s="3"/>
       <c r="F254" s="3"/>
       <c r="J254" s="3"/>
-      <c r="L254" s="3"/>
-      <c r="M254" s="3"/>
-    </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="2"/>
       <c r="B255" s="2"/>
       <c r="C255" s="3"/>
       <c r="F255" s="3"/>
       <c r="J255" s="3"/>
-      <c r="L255" s="3"/>
-      <c r="M255" s="3"/>
-    </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="2"/>
       <c r="B256" s="2"/>
       <c r="C256" s="3"/>
       <c r="F256" s="3"/>
       <c r="J256" s="3"/>
-      <c r="L256" s="3"/>
-      <c r="M256" s="3"/>
-    </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="2"/>
       <c r="B257" s="2"/>
       <c r="C257" s="3"/>
       <c r="F257" s="3"/>
       <c r="J257" s="3"/>
-      <c r="L257" s="3"/>
-      <c r="M257" s="3"/>
-    </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="2"/>
       <c r="B258" s="2"/>
       <c r="C258" s="3"/>
       <c r="F258" s="3"/>
       <c r="J258" s="3"/>
-      <c r="L258" s="3"/>
-      <c r="M258" s="3"/>
-    </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="2"/>
       <c r="B259" s="2"/>
       <c r="C259" s="3"/>
       <c r="F259" s="3"/>
       <c r="J259" s="3"/>
-      <c r="L259" s="3"/>
-      <c r="M259" s="3"/>
-    </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="2"/>
       <c r="B260" s="2"/>
       <c r="C260" s="3"/>
       <c r="F260" s="3"/>
       <c r="J260" s="3"/>
-      <c r="L260" s="3"/>
-      <c r="M260" s="3"/>
-    </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="2"/>
       <c r="B261" s="2"/>
       <c r="C261" s="3"/>
       <c r="F261" s="3"/>
       <c r="J261" s="3"/>
-      <c r="L261" s="3"/>
-      <c r="M261" s="3"/>
-    </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="2"/>
       <c r="B262" s="2"/>
       <c r="C262" s="3"/>
       <c r="F262" s="3"/>
       <c r="J262" s="3"/>
-      <c r="L262" s="3"/>
-      <c r="M262" s="3"/>
-    </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="2"/>
       <c r="B263" s="2"/>
       <c r="C263" s="3"/>
       <c r="F263" s="3"/>
       <c r="J263" s="3"/>
-      <c r="L263" s="3"/>
-      <c r="M263" s="3"/>
-    </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="2"/>
       <c r="B264" s="2"/>
       <c r="C264" s="3"/>
       <c r="F264" s="3"/>
       <c r="J264" s="3"/>
-      <c r="L264" s="3"/>
-      <c r="M264" s="3"/>
-    </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="2"/>
       <c r="B265" s="2"/>
       <c r="C265" s="3"/>
       <c r="F265" s="3"/>
       <c r="J265" s="3"/>
-      <c r="L265" s="3"/>
-      <c r="M265" s="3"/>
-    </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="2"/>
       <c r="B266" s="2"/>
       <c r="C266" s="3"/>
       <c r="F266" s="3"/>
       <c r="J266" s="3"/>
-      <c r="L266" s="3"/>
-      <c r="M266" s="3"/>
-    </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="2"/>
       <c r="B267" s="2"/>
       <c r="C267" s="3"/>
       <c r="F267" s="3"/>
       <c r="J267" s="3"/>
-      <c r="L267" s="3"/>
-      <c r="M267" s="3"/>
-    </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="2"/>
       <c r="B268" s="2"/>
       <c r="C268" s="3"/>
       <c r="F268" s="3"/>
       <c r="J268" s="3"/>
-      <c r="L268" s="3"/>
-      <c r="M268" s="3"/>
-    </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="2"/>
       <c r="B269" s="2"/>
       <c r="C269" s="3"/>
       <c r="F269" s="3"/>
       <c r="J269" s="3"/>
-      <c r="L269" s="3"/>
-      <c r="M269" s="3"/>
-    </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="2"/>
       <c r="B270" s="2"/>
       <c r="C270" s="3"/>
       <c r="F270" s="3"/>
       <c r="J270" s="3"/>
-      <c r="L270" s="3"/>
-      <c r="M270" s="3"/>
-    </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="2"/>
       <c r="B271" s="2"/>
       <c r="C271" s="3"/>
       <c r="F271" s="3"/>
       <c r="J271" s="3"/>
-      <c r="L271" s="3"/>
-      <c r="M271" s="3"/>
-    </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="2"/>
       <c r="B272" s="2"/>
       <c r="C272" s="3"/>
       <c r="F272" s="3"/>
       <c r="J272" s="3"/>
-      <c r="L272" s="3"/>
-      <c r="M272" s="3"/>
-    </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="2"/>
       <c r="B273" s="2"/>
       <c r="C273" s="3"/>
       <c r="F273" s="3"/>
       <c r="J273" s="3"/>
-      <c r="L273" s="3"/>
-      <c r="M273" s="3"/>
-    </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="2"/>
       <c r="B274" s="2"/>
       <c r="C274" s="3"/>
       <c r="F274" s="3"/>
       <c r="J274" s="3"/>
-      <c r="L274" s="3"/>
-      <c r="M274" s="3"/>
-    </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="2"/>
       <c r="B275" s="2"/>
       <c r="C275" s="3"/>
       <c r="F275" s="3"/>
       <c r="J275" s="3"/>
-      <c r="L275" s="3"/>
-      <c r="M275" s="3"/>
-    </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="2"/>
       <c r="B276" s="2"/>
       <c r="C276" s="3"/>
       <c r="F276" s="3"/>
       <c r="J276" s="3"/>
-      <c r="L276" s="3"/>
-      <c r="M276" s="3"/>
-    </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="2"/>
       <c r="B277" s="2"/>
       <c r="C277" s="3"/>
       <c r="F277" s="3"/>
       <c r="J277" s="3"/>
-      <c r="L277" s="3"/>
-      <c r="M277" s="3"/>
-    </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="2"/>
       <c r="B278" s="2"/>
       <c r="C278" s="3"/>
       <c r="F278" s="3"/>
       <c r="J278" s="3"/>
-      <c r="L278" s="3"/>
-      <c r="M278" s="3"/>
-    </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="2"/>
       <c r="B279" s="2"/>
       <c r="C279" s="3"/>
       <c r="F279" s="3"/>
       <c r="J279" s="3"/>
-      <c r="L279" s="3"/>
-      <c r="M279" s="3"/>
-    </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="2"/>
       <c r="B280" s="2"/>
       <c r="C280" s="3"/>
       <c r="F280" s="3"/>
       <c r="J280" s="3"/>
-      <c r="L280" s="3"/>
-      <c r="M280" s="3"/>
-    </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="2"/>
       <c r="B281" s="2"/>
       <c r="C281" s="3"/>
       <c r="F281" s="3"/>
       <c r="J281" s="3"/>
-      <c r="L281" s="3"/>
-      <c r="M281" s="3"/>
-    </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="2"/>
       <c r="B282" s="2"/>
       <c r="C282" s="3"/>
       <c r="F282" s="3"/>
       <c r="J282" s="3"/>
-      <c r="L282" s="3"/>
-      <c r="M282" s="3"/>
-    </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="2"/>
       <c r="B283" s="2"/>
       <c r="C283" s="3"/>
       <c r="F283" s="3"/>
       <c r="J283" s="3"/>
-      <c r="L283" s="3"/>
-      <c r="M283" s="3"/>
-    </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="2"/>
       <c r="B284" s="2"/>
       <c r="C284" s="3"/>
       <c r="F284" s="3"/>
       <c r="J284" s="3"/>
-      <c r="L284" s="3"/>
-      <c r="M284" s="3"/>
-    </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="2"/>
       <c r="B285" s="2"/>
       <c r="C285" s="3"/>
       <c r="F285" s="3"/>
       <c r="J285" s="3"/>
-      <c r="L285" s="3"/>
-      <c r="M285" s="3"/>
-    </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="2"/>
       <c r="B286" s="2"/>
       <c r="C286" s="3"/>
       <c r="F286" s="3"/>
       <c r="J286" s="3"/>
-      <c r="L286" s="3"/>
-      <c r="M286" s="3"/>
-    </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="2"/>
       <c r="B287" s="2"/>
       <c r="C287" s="3"/>
       <c r="F287" s="3"/>
       <c r="J287" s="3"/>
-      <c r="L287" s="3"/>
-      <c r="M287" s="3"/>
-    </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="2"/>
       <c r="B288" s="2"/>
       <c r="C288" s="3"/>
       <c r="F288" s="3"/>
       <c r="J288" s="3"/>
-      <c r="L288" s="3"/>
-      <c r="M288" s="3"/>
-    </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="2"/>
       <c r="B289" s="2"/>
       <c r="C289" s="3"/>
       <c r="F289" s="3"/>
       <c r="J289" s="3"/>
-      <c r="L289" s="3"/>
-      <c r="M289" s="3"/>
-    </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="2"/>
       <c r="B290" s="2"/>
       <c r="C290" s="3"/>
       <c r="F290" s="3"/>
       <c r="J290" s="3"/>
-      <c r="L290" s="3"/>
-      <c r="M290" s="3"/>
-    </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="2"/>
       <c r="B291" s="2"/>
       <c r="C291" s="3"/>
       <c r="F291" s="3"/>
       <c r="J291" s="3"/>
-      <c r="L291" s="3"/>
-      <c r="M291" s="3"/>
-    </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="2"/>
       <c r="B292" s="2"/>
       <c r="C292" s="3"/>
       <c r="F292" s="3"/>
       <c r="J292" s="3"/>
-      <c r="L292" s="3"/>
-      <c r="M292" s="3"/>
-    </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="2"/>
       <c r="B293" s="2"/>
       <c r="C293" s="3"/>
       <c r="F293" s="3"/>
       <c r="J293" s="3"/>
-      <c r="L293" s="3"/>
-      <c r="M293" s="3"/>
-    </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="2"/>
       <c r="B294" s="2"/>
       <c r="C294" s="3"/>
       <c r="F294" s="3"/>
       <c r="J294" s="3"/>
-      <c r="L294" s="3"/>
-      <c r="M294" s="3"/>
-    </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="2"/>
       <c r="B295" s="2"/>
       <c r="C295" s="3"/>
       <c r="F295" s="3"/>
       <c r="J295" s="3"/>
-      <c r="L295" s="3"/>
-      <c r="M295" s="3"/>
-    </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="2"/>
       <c r="B296" s="2"/>
       <c r="C296" s="3"/>
       <c r="F296" s="3"/>
       <c r="J296" s="3"/>
-      <c r="L296" s="3"/>
-      <c r="M296" s="3"/>
-    </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="2"/>
       <c r="B297" s="2"/>
       <c r="C297" s="3"/>
       <c r="F297" s="3"/>
       <c r="J297" s="3"/>
-      <c r="L297" s="3"/>
-      <c r="M297" s="3"/>
-    </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="2"/>
       <c r="B298" s="2"/>
       <c r="C298" s="3"/>
       <c r="F298" s="3"/>
       <c r="J298" s="3"/>
-      <c r="L298" s="3"/>
-      <c r="M298" s="3"/>
-    </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" s="2"/>
       <c r="B299" s="2"/>
       <c r="C299" s="3"/>
       <c r="F299" s="3"/>
       <c r="J299" s="3"/>
-      <c r="L299" s="3"/>
-      <c r="M299" s="3"/>
-    </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" s="2"/>
       <c r="B300" s="2"/>
       <c r="C300" s="3"/>
       <c r="F300" s="3"/>
       <c r="J300" s="3"/>
-      <c r="L300" s="3"/>
-      <c r="M300" s="3"/>
-    </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="2"/>
       <c r="B301" s="2"/>
       <c r="C301" s="3"/>
       <c r="F301" s="3"/>
       <c r="J301" s="3"/>
-      <c r="L301" s="3"/>
-      <c r="M301" s="3"/>
-    </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="2"/>
       <c r="B302" s="2"/>
       <c r="C302" s="3"/>
       <c r="F302" s="3"/>
       <c r="J302" s="3"/>
-      <c r="L302" s="3"/>
-      <c r="M302" s="3"/>
-    </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="2"/>
       <c r="B303" s="2"/>
       <c r="C303" s="3"/>
       <c r="F303" s="3"/>
       <c r="J303" s="3"/>
-      <c r="L303" s="3"/>
-      <c r="M303" s="3"/>
-    </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="2"/>
       <c r="B304" s="2"/>
       <c r="C304" s="3"/>
       <c r="F304" s="3"/>
       <c r="J304" s="3"/>
-      <c r="L304" s="3"/>
-      <c r="M304" s="3"/>
-    </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" s="2"/>
       <c r="B305" s="2"/>
       <c r="C305" s="3"/>
       <c r="F305" s="3"/>
       <c r="J305" s="3"/>
-      <c r="L305" s="3"/>
-      <c r="M305" s="3"/>
-    </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" s="2"/>
       <c r="B306" s="2"/>
       <c r="C306" s="3"/>
       <c r="F306" s="3"/>
       <c r="J306" s="3"/>
-      <c r="L306" s="3"/>
-      <c r="M306" s="3"/>
-    </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" s="2"/>
       <c r="B307" s="2"/>
       <c r="C307" s="3"/>
       <c r="F307" s="3"/>
       <c r="J307" s="3"/>
-      <c r="L307" s="3"/>
-      <c r="M307" s="3"/>
-    </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" s="2"/>
       <c r="B308" s="2"/>
       <c r="C308" s="3"/>
       <c r="F308" s="3"/>
       <c r="J308" s="3"/>
-      <c r="L308" s="3"/>
-      <c r="M308" s="3"/>
-    </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" s="2"/>
       <c r="B309" s="2"/>
       <c r="C309" s="3"/>
       <c r="F309" s="3"/>
       <c r="J309" s="3"/>
-      <c r="L309" s="3"/>
-      <c r="M309" s="3"/>
-    </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" s="2"/>
       <c r="B310" s="2"/>
       <c r="C310" s="3"/>
       <c r="F310" s="3"/>
       <c r="J310" s="3"/>
-      <c r="L310" s="3"/>
-      <c r="M310" s="3"/>
-    </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" s="2"/>
       <c r="B311" s="2"/>
       <c r="C311" s="3"/>
       <c r="F311" s="3"/>
       <c r="J311" s="3"/>
-      <c r="L311" s="3"/>
-      <c r="M311" s="3"/>
-    </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" s="2"/>
       <c r="B312" s="2"/>
       <c r="C312" s="3"/>
       <c r="F312" s="3"/>
       <c r="J312" s="3"/>
-      <c r="L312" s="3"/>
-      <c r="M312" s="3"/>
-    </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" s="2"/>
       <c r="B313" s="2"/>
       <c r="C313" s="3"/>
       <c r="F313" s="3"/>
       <c r="J313" s="3"/>
-      <c r="L313" s="3"/>
-      <c r="M313" s="3"/>
-    </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" s="2"/>
       <c r="B314" s="2"/>
       <c r="C314" s="3"/>
       <c r="F314" s="3"/>
       <c r="J314" s="3"/>
-      <c r="L314" s="3"/>
-      <c r="M314" s="3"/>
-    </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" s="2"/>
       <c r="B315" s="2"/>
       <c r="C315" s="3"/>
       <c r="F315" s="3"/>
       <c r="J315" s="3"/>
-      <c r="L315" s="3"/>
-      <c r="M315" s="3"/>
-    </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" s="2"/>
       <c r="B316" s="2"/>
       <c r="C316" s="3"/>
       <c r="F316" s="3"/>
       <c r="J316" s="3"/>
-      <c r="L316" s="3"/>
-      <c r="M316" s="3"/>
-    </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" s="2"/>
       <c r="B317" s="2"/>
       <c r="C317" s="3"/>
       <c r="F317" s="3"/>
       <c r="J317" s="3"/>
-      <c r="L317" s="3"/>
-      <c r="M317" s="3"/>
-    </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" s="2"/>
       <c r="B318" s="2"/>
       <c r="C318" s="3"/>
       <c r="F318" s="3"/>
       <c r="J318" s="3"/>
-      <c r="L318" s="3"/>
-      <c r="M318" s="3"/>
-    </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" s="2"/>
       <c r="B319" s="2"/>
       <c r="C319" s="3"/>
       <c r="F319" s="3"/>
       <c r="J319" s="3"/>
-      <c r="L319" s="3"/>
-      <c r="M319" s="3"/>
-    </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" s="2"/>
       <c r="B320" s="2"/>
       <c r="C320" s="3"/>
       <c r="F320" s="3"/>
       <c r="J320" s="3"/>
-      <c r="L320" s="3"/>
-      <c r="M320" s="3"/>
-    </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321" s="2"/>
       <c r="B321" s="2"/>
       <c r="C321" s="3"/>
       <c r="F321" s="3"/>
       <c r="J321" s="3"/>
-      <c r="L321" s="3"/>
-      <c r="M321" s="3"/>
-    </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322" s="2"/>
       <c r="B322" s="2"/>
       <c r="C322" s="3"/>
       <c r="F322" s="3"/>
       <c r="J322" s="3"/>
-      <c r="L322" s="3"/>
-      <c r="M322" s="3"/>
-    </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" s="2"/>
       <c r="B323" s="2"/>
       <c r="C323" s="3"/>
       <c r="F323" s="3"/>
       <c r="J323" s="3"/>
-      <c r="L323" s="3"/>
-      <c r="M323" s="3"/>
-    </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324" s="2"/>
       <c r="B324" s="2"/>
       <c r="C324" s="3"/>
       <c r="F324" s="3"/>
       <c r="J324" s="3"/>
-      <c r="L324" s="3"/>
-      <c r="M324" s="3"/>
-    </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325" s="2"/>
       <c r="B325" s="2"/>
       <c r="C325" s="3"/>
       <c r="F325" s="3"/>
       <c r="J325" s="3"/>
-      <c r="L325" s="3"/>
-      <c r="M325" s="3"/>
-    </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326" s="2"/>
       <c r="B326" s="2"/>
       <c r="C326" s="3"/>
       <c r="F326" s="3"/>
       <c r="J326" s="3"/>
-      <c r="L326" s="3"/>
-      <c r="M326" s="3"/>
-    </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327" s="2"/>
       <c r="B327" s="2"/>
       <c r="C327" s="3"/>
       <c r="F327" s="3"/>
       <c r="J327" s="3"/>
-      <c r="L327" s="3"/>
-      <c r="M327" s="3"/>
-    </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328" s="2"/>
       <c r="B328" s="2"/>
       <c r="C328" s="3"/>
       <c r="F328" s="3"/>
       <c r="J328" s="3"/>
-      <c r="L328" s="3"/>
-      <c r="M328" s="3"/>
-    </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329" s="2"/>
       <c r="B329" s="2"/>
       <c r="C329" s="3"/>
       <c r="F329" s="3"/>
       <c r="J329" s="3"/>
-      <c r="L329" s="3"/>
-      <c r="M329" s="3"/>
-    </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" s="2"/>
       <c r="B330" s="2"/>
       <c r="C330" s="3"/>
       <c r="F330" s="3"/>
       <c r="J330" s="3"/>
-      <c r="L330" s="3"/>
-      <c r="M330" s="3"/>
-    </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" s="2"/>
       <c r="B331" s="2"/>
       <c r="C331" s="3"/>
       <c r="F331" s="3"/>
       <c r="J331" s="3"/>
-      <c r="L331" s="3"/>
-      <c r="M331" s="3"/>
-    </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332" s="2"/>
       <c r="B332" s="2"/>
       <c r="C332" s="3"/>
       <c r="F332" s="3"/>
       <c r="J332" s="3"/>
-      <c r="L332" s="3"/>
-      <c r="M332" s="3"/>
-    </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" s="2"/>
       <c r="B333" s="2"/>
       <c r="C333" s="3"/>
       <c r="F333" s="3"/>
       <c r="J333" s="3"/>
-      <c r="L333" s="3"/>
-      <c r="M333" s="3"/>
-    </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334" s="2"/>
       <c r="B334" s="2"/>
       <c r="C334" s="3"/>
       <c r="F334" s="3"/>
       <c r="J334" s="3"/>
-      <c r="L334" s="3"/>
-      <c r="M334" s="3"/>
-    </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335" s="2"/>
       <c r="B335" s="2"/>
       <c r="C335" s="3"/>
       <c r="F335" s="3"/>
       <c r="J335" s="3"/>
-      <c r="L335" s="3"/>
-      <c r="M335" s="3"/>
-    </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336" s="2"/>
       <c r="B336" s="2"/>
       <c r="C336" s="3"/>
       <c r="F336" s="3"/>
       <c r="J336" s="3"/>
-      <c r="L336" s="3"/>
-      <c r="M336" s="3"/>
-    </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337" s="2"/>
       <c r="B337" s="2"/>
       <c r="C337" s="3"/>
       <c r="F337" s="3"/>
       <c r="J337" s="3"/>
-      <c r="L337" s="3"/>
-      <c r="M337" s="3"/>
-    </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338" s="2"/>
       <c r="B338" s="2"/>
       <c r="C338" s="3"/>
       <c r="F338" s="3"/>
       <c r="J338" s="3"/>
-      <c r="L338" s="3"/>
-      <c r="M338" s="3"/>
-    </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339" s="2"/>
       <c r="B339" s="2"/>
       <c r="C339" s="3"/>
       <c r="F339" s="3"/>
       <c r="J339" s="3"/>
-      <c r="L339" s="3"/>
-      <c r="M339" s="3"/>
-    </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340" s="2"/>
       <c r="B340" s="2"/>
       <c r="C340" s="3"/>
       <c r="F340" s="3"/>
       <c r="J340" s="3"/>
-      <c r="L340" s="3"/>
-      <c r="M340" s="3"/>
-    </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341" s="2"/>
       <c r="B341" s="2"/>
       <c r="C341" s="3"/>
       <c r="F341" s="3"/>
       <c r="J341" s="3"/>
-      <c r="L341" s="3"/>
-      <c r="M341" s="3"/>
-    </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" s="2"/>
       <c r="B342" s="2"/>
       <c r="C342" s="3"/>
       <c r="F342" s="3"/>
       <c r="J342" s="3"/>
-      <c r="L342" s="3"/>
-      <c r="M342" s="3"/>
-    </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" s="2"/>
       <c r="B343" s="2"/>
       <c r="C343" s="3"/>
       <c r="F343" s="3"/>
       <c r="J343" s="3"/>
-      <c r="L343" s="3"/>
-      <c r="M343" s="3"/>
-    </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344" s="2"/>
       <c r="B344" s="2"/>
       <c r="C344" s="3"/>
       <c r="F344" s="3"/>
       <c r="J344" s="3"/>
-      <c r="L344" s="3"/>
-      <c r="M344" s="3"/>
-    </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345" s="2"/>
       <c r="B345" s="2"/>
       <c r="C345" s="3"/>
       <c r="F345" s="3"/>
       <c r="J345" s="3"/>
-      <c r="L345" s="3"/>
-      <c r="M345" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M103" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>